<commit_message>
Enhance output readability in optimization and regression scripts
- In `optimization.py`, added section headers for optimized weights, performance metrics, and exposure differences to improve clarity of printed results.
- Updated print statements to include headers and formatted output for better understanding of the results.
- In `regression.py`, added headers to the printed exposure, p-values, and significant exposure data, and limited output to the first row for brevity.
- Added type ignore comments for potential type issues in factor regression calls.
</commit_message>
<xml_diff>
--- a/final report/data/stock_list.xlsx
+++ b/final report/data/stock_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eric/Developer/fin_model_1/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eric/Documents/study/rutgers/semester 2/financial modelling 1/fin_model_1/final report/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E79D0E87-62FF-2A44-8CA4-C6ADF8CC7EBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{154C2470-EFF4-834E-8FD6-FEEC5100DCA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="500" windowWidth="25600" windowHeight="31500" xr2:uid="{59FA3E77-6D31-314F-933E-2951A66676F8}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{59FA3E77-6D31-314F-933E-2951A66676F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">2</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="93">
   <si>
     <t>Company</t>
   </si>
@@ -871,6 +871,27 @@
   </si>
   <si>
     <t>Weight</t>
+  </si>
+  <si>
+    <t>Shares</t>
+  </si>
+  <si>
+    <t>Transaction Cost</t>
+  </si>
+  <si>
+    <t>Value of Shares</t>
+  </si>
+  <si>
+    <t>Target Weight</t>
+  </si>
+  <si>
+    <t>13 WEEK TREASURY BILL</t>
+  </si>
+  <si>
+    <t>^IRX</t>
+  </si>
+  <si>
+    <t>T-bills</t>
   </si>
 </sst>
 </file>
@@ -945,13 +966,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1287,19 +1307,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DC1370C-9E24-DB43-A6B1-7D879DB15B65}">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.83203125"/>
+    <col min="9" max="9" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1318,10 +1341,23 @@
       <c r="F1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G1" s="1">
+        <v>20250131</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>18</v>
       </c>
@@ -1337,11 +1373,29 @@
       <c r="E2">
         <v>14593</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2">
+        <f>I2/1000800</f>
+        <v>4.0795363709032771E-2</v>
+      </c>
+      <c r="G2">
+        <v>236</v>
+      </c>
+      <c r="H2">
+        <v>173</v>
+      </c>
+      <c r="I2">
+        <f>G2*H2</f>
+        <v>40828</v>
+      </c>
+      <c r="J2">
+        <f>I2*0.002</f>
+        <v>81.656000000000006</v>
+      </c>
+      <c r="K2" s="4">
         <v>4.0899999999999999E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -1357,11 +1411,29 @@
       <c r="E3">
         <v>14008</v>
       </c>
-      <c r="F3" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F3">
+        <f t="shared" ref="F3:F32" si="0">I3/1000800</f>
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>285.42</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I31" si="1">G3*H3</f>
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J31" si="2">I3*0.002</f>
+        <v>0</v>
+      </c>
+      <c r="K3" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
@@ -1377,11 +1449,29 @@
       <c r="E4">
         <v>84788</v>
       </c>
-      <c r="F4" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>237.68</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K4" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1397,11 +1487,29 @@
       <c r="E5">
         <v>59176</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>4.1869904076738608E-2</v>
+      </c>
+      <c r="G5">
+        <v>317.45</v>
+      </c>
+      <c r="H5">
+        <v>132</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>41903.4</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="2"/>
+        <v>83.80680000000001</v>
+      </c>
+      <c r="K5" s="4">
         <v>4.1799999999999997E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>21</v>
       </c>
@@ -1417,11 +1525,29 @@
       <c r="E6">
         <v>19561</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>2.2223741007194243E-2</v>
+      </c>
+      <c r="G6">
+        <v>176.52</v>
+      </c>
+      <c r="H6">
+        <v>126</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>22241.52</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="2"/>
+        <v>44.483040000000003</v>
+      </c>
+      <c r="K6" s="4">
         <v>2.23E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>24</v>
       </c>
@@ -1437,11 +1563,29 @@
       <c r="E7">
         <v>18542</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>8.9816626698641086E-2</v>
+      </c>
+      <c r="G7">
+        <v>371.44</v>
+      </c>
+      <c r="H7">
+        <v>242</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="1"/>
+        <v>89888.48</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="2"/>
+        <v>179.77696</v>
+      </c>
+      <c r="K7" s="4">
         <v>9.0200000000000002E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>66</v>
       </c>
@@ -1457,11 +1601,29 @@
       <c r="E8">
         <v>90215</v>
       </c>
-      <c r="F8" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>341.7</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K8" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>30</v>
       </c>
@@ -1477,11 +1639,29 @@
       <c r="E9">
         <v>76076</v>
       </c>
-      <c r="F9" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>60.6</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K9" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>27</v>
       </c>
@@ -1497,11 +1677,29 @@
       <c r="E10">
         <v>14541</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>9.9877398081534771E-2</v>
+      </c>
+      <c r="G10">
+        <v>149.19</v>
+      </c>
+      <c r="H10">
+        <v>670</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="1"/>
+        <v>99957.3</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="2"/>
+        <v>199.91460000000001</v>
+      </c>
+      <c r="K10" s="4">
         <v>0.1</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>35</v>
       </c>
@@ -1517,11 +1715,29 @@
       <c r="E11">
         <v>26403</v>
       </c>
-      <c r="F11" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>113.06</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K11" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>38</v>
       </c>
@@ -1537,11 +1753,29 @@
       <c r="E12">
         <v>86868</v>
       </c>
-      <c r="F12" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>640.4</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K12" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>40</v>
       </c>
@@ -1557,11 +1791,29 @@
       <c r="E13">
         <v>66181</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>5.3514588329336532E-2</v>
+      </c>
+      <c r="G13">
+        <v>411.98</v>
+      </c>
+      <c r="H13">
+        <v>130</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="1"/>
+        <v>53557.4</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="2"/>
+        <v>107.1148</v>
+      </c>
+      <c r="K13" s="4">
         <v>5.3900000000000003E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>43</v>
       </c>
@@ -1577,11 +1829,29 @@
       <c r="E14">
         <v>10145</v>
       </c>
-      <c r="F14" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>223.72</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K14" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>45</v>
       </c>
@@ -1597,11 +1867,29 @@
       <c r="E15">
         <v>12490</v>
       </c>
-      <c r="F15" s="4">
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>0.100154276578737</v>
+      </c>
+      <c r="G15">
+        <v>255.7</v>
+      </c>
+      <c r="H15">
+        <v>392</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="1"/>
+        <v>100234.4</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="2"/>
+        <v>200.46879999999999</v>
+      </c>
+      <c r="K15" s="4">
         <v>0.1</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>46</v>
       </c>
@@ -1617,11 +1905,29 @@
       <c r="E16">
         <v>22111</v>
       </c>
-      <c r="F16" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>152.15</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K16" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>49</v>
       </c>
@@ -1637,11 +1943,29 @@
       <c r="E17">
         <v>47896</v>
       </c>
-      <c r="F17" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>267.3</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K17" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>32</v>
       </c>
@@ -1657,11 +1981,29 @@
       <c r="E18">
         <v>11308</v>
       </c>
-      <c r="F18" s="4">
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>9.996450839328537E-2</v>
+      </c>
+      <c r="G18">
+        <v>63.48</v>
+      </c>
+      <c r="H18">
+        <v>1576</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="1"/>
+        <v>100044.48</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="2"/>
+        <v>200.08895999999999</v>
+      </c>
+      <c r="K18" s="4">
         <v>0.1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>51</v>
       </c>
@@ -1677,11 +2019,29 @@
       <c r="E19">
         <v>43449</v>
       </c>
-      <c r="F19" s="4">
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>9.9810351718625095E-2</v>
+      </c>
+      <c r="G19">
+        <v>288.7</v>
+      </c>
+      <c r="H19">
+        <v>346</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="1"/>
+        <v>99890.2</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="2"/>
+        <v>199.78039999999999</v>
+      </c>
+      <c r="K19" s="4">
         <v>0.1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>4</v>
       </c>
@@ -1697,11 +2057,29 @@
       <c r="E20">
         <v>22592</v>
       </c>
-      <c r="F20" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>152.19999999999999</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K20" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>54</v>
       </c>
@@ -1717,11 +2095,29 @@
       <c r="E21">
         <v>22752</v>
       </c>
-      <c r="F21" s="4">
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>9.9728417266187044E-2</v>
+      </c>
+      <c r="G21">
+        <v>98.82</v>
+      </c>
+      <c r="H21">
+        <v>1010</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="1"/>
+        <v>99808.2</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="2"/>
+        <v>199.6164</v>
+      </c>
+      <c r="K21" s="4">
         <v>0.1</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>56</v>
       </c>
@@ -1737,11 +2133,29 @@
       <c r="E22">
         <v>10107</v>
       </c>
-      <c r="F22" s="4">
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>7.3406894484412469E-2</v>
+      </c>
+      <c r="G22">
+        <v>415.06</v>
+      </c>
+      <c r="H22">
+        <v>177</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="1"/>
+        <v>73465.62</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="2"/>
+        <v>146.93124</v>
+      </c>
+      <c r="K22" s="4">
         <v>7.3599999999999999E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>58</v>
       </c>
@@ -1757,11 +2171,29 @@
       <c r="E23">
         <v>57665</v>
       </c>
-      <c r="F23" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>76.900000000000006</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K23" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>61</v>
       </c>
@@ -1777,11 +2209,29 @@
       <c r="E24">
         <v>86580</v>
       </c>
-      <c r="F24" s="4">
+      <c r="F24">
+        <f t="shared" si="0"/>
+        <v>5.0029166666666659E-2</v>
+      </c>
+      <c r="G24">
+        <v>120.07</v>
+      </c>
+      <c r="H24">
+        <v>417</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="1"/>
+        <v>50069.189999999995</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="2"/>
+        <v>100.13838</v>
+      </c>
+      <c r="K24" s="4">
         <v>5.0099999999999999E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>63</v>
       </c>
@@ -1797,11 +2247,29 @@
       <c r="E25">
         <v>18163</v>
       </c>
-      <c r="F25" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>165.99</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K25" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>68</v>
       </c>
@@ -1817,11 +2285,29 @@
       <c r="E26">
         <v>36468</v>
       </c>
-      <c r="F26" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>358.16</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K26" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>71</v>
       </c>
@@ -1837,11 +2323,29 @@
       <c r="E27">
         <v>59459</v>
       </c>
-      <c r="F27" s="4">
+      <c r="F27">
+        <f t="shared" si="0"/>
+        <v>9.9708493205435664E-2</v>
+      </c>
+      <c r="G27">
+        <v>245.18</v>
+      </c>
+      <c r="H27">
+        <v>407</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="1"/>
+        <v>99788.260000000009</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="2"/>
+        <v>199.57652000000002</v>
+      </c>
+      <c r="K27" s="4">
         <v>0.1</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>74</v>
       </c>
@@ -1857,12 +2361,29 @@
       <c r="E28">
         <v>92655</v>
       </c>
-      <c r="F28" s="4">
+      <c r="F28">
+        <f t="shared" si="0"/>
+        <v>2.7102817745803358E-2</v>
+      </c>
+      <c r="G28">
+        <v>542.49</v>
+      </c>
+      <c r="H28">
+        <v>50</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="1"/>
+        <v>27124.5</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="2"/>
+        <v>54.249000000000002</v>
+      </c>
+      <c r="K28" s="4">
         <v>2.7300000000000001E-2</v>
       </c>
-      <c r="G28" s="2"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>80</v>
       </c>
@@ -1878,11 +2399,29 @@
       <c r="E29">
         <v>92611</v>
       </c>
-      <c r="F29" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>341.8</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K29" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>77</v>
       </c>
@@ -1898,11 +2437,29 @@
       <c r="E30">
         <v>65875</v>
       </c>
-      <c r="F30" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>39.39</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K30" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>82</v>
       </c>
@@ -1918,7 +2475,47 @@
       <c r="E31">
         <v>55976</v>
       </c>
-      <c r="F31" s="4">
+      <c r="F31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>98.16</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K31" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="0"/>
+        <v>1.4469424462059026E-6</v>
+      </c>
+      <c r="I32">
+        <f>1000800 - SUM(I2:I31)-SUM(J2:J31)</f>
+        <v>1.4481000001628672</v>
+      </c>
+      <c r="K32" s="4">
         <v>0</v>
       </c>
     </row>
@@ -1929,5 +2526,6 @@
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>